<commit_message>
Fixed bug when writing data to a spreadsheet.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -17535,11 +17535,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18104,637 +18104,12 @@
       <c r="U9" s="5"/>
       <c r="V9" s="60"/>
     </row>
-    <row r="10" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="220"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="110">
-        <v>3</v>
-      </c>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="60"/>
-    </row>
-    <row r="11" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="220"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="110">
-        <v>4</v>
-      </c>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="60"/>
-    </row>
-    <row r="12" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="220"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="110">
-        <v>5</v>
-      </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="60"/>
-    </row>
-    <row r="13" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="220"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="110">
-        <v>6</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="60"/>
-    </row>
-    <row r="14" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="220"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="110">
-        <v>7</v>
-      </c>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="60"/>
-    </row>
-    <row r="15" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="220"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="110">
-        <v>8</v>
-      </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="60"/>
-    </row>
-    <row r="16" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="220"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="110">
-        <v>9</v>
-      </c>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="60"/>
-    </row>
-    <row r="17" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="220"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="110">
-        <v>10</v>
-      </c>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="60"/>
-    </row>
-    <row r="18" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="220"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="110">
-        <v>11</v>
-      </c>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="60"/>
-    </row>
-    <row r="19" spans="1:22" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="220"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="110">
-        <v>12</v>
-      </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="60"/>
-    </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="220"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="110">
-        <v>13</v>
-      </c>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="60"/>
-    </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="220"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="110">
-        <v>14</v>
-      </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="60"/>
-    </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="220"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="110">
-        <v>15</v>
-      </c>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="60"/>
-    </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="220"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="110">
-        <v>16</v>
-      </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="60"/>
-    </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="220"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="110">
-        <v>17</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="60"/>
-    </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="220"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="110">
-        <v>18</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="60"/>
-    </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="220"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="110">
-        <v>19</v>
-      </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="60"/>
-    </row>
-    <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="220"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="110">
-        <v>20</v>
-      </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="60"/>
-    </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="220"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="110">
-        <v>21</v>
-      </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="60"/>
-    </row>
-    <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="220"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="110">
-        <v>22</v>
-      </c>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="60"/>
-    </row>
-    <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="220"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="110">
-        <v>23</v>
-      </c>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="60"/>
-    </row>
-    <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="220"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="110">
-        <v>24</v>
-      </c>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="60"/>
-    </row>
-    <row r="32" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="220"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="110">
-        <v>25</v>
-      </c>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="60"/>
-    </row>
-    <row r="33" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="220"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="110">
-        <v>26</v>
-      </c>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="60"/>
-    </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A8:H33" name="Område1_3"/>
-    <protectedRange sqref="M20:O33" name="Område1"/>
-    <protectedRange sqref="I8:L33" name="Område1_1"/>
-    <protectedRange sqref="P19:P33 N19:O19 N8:P18" name="Område1_1_1"/>
-    <protectedRange sqref="M8:M19" name="Område1_2"/>
+    <protectedRange sqref="A8:H9" name="Område1_3"/>
+    <protectedRange sqref="I8:L9" name="Område1_1"/>
+    <protectedRange sqref="N8:P9" name="Område1_1_1"/>
+    <protectedRange sqref="M8:M9" name="Område1_2"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -24805,7 +24180,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'[TestSheet.xlsx]SSNN Reference Data'!#REF!</xm:f>
+            <xm:f>'C:\Projects\AnNaSpreadSheetParser\src\AnNaSpreadsheetParser.Test\[TestSheet.xlsx]SSNN Reference Data'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E15:E24</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
Added support for Cruise sheet.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arrival_Or_Departure" sheetId="2" r:id="rId1"/>
@@ -2214,7 +2214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="1394">
   <si>
     <t>Port call</t>
   </si>
@@ -8189,7 +8189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -9036,6 +9036,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -16978,9 +16986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17187,9 +17195,15 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
+      <c r="A8" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B8" s="224">
+        <v>42685</v>
+      </c>
+      <c r="C8" s="225">
+        <v>0.46597222222222223</v>
+      </c>
       <c r="D8" s="78"/>
       <c r="E8" s="81"/>
       <c r="F8" s="116"/>
@@ -17537,7 +17551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>

</xml_diff>

<commit_message>
Added support for applying type hints to GetValueAt(). Also added a hack to remove empty rows from bulk data to improve performance.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Arrival_Or_Departure" sheetId="2" r:id="rId1"/>
@@ -2214,7 +2214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="1417">
   <si>
     <t>Port call</t>
   </si>
@@ -7174,6 +7174,75 @@
   </si>
   <si>
     <t>Navigator</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Olsen</t>
+  </si>
+  <si>
+    <t>Ira</t>
+  </si>
+  <si>
+    <t>Mercer</t>
+  </si>
+  <si>
+    <t>Gothenburg</t>
+  </si>
+  <si>
+    <t>Uriel</t>
+  </si>
+  <si>
+    <t>Shannon</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>NOSVG</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>01.01.2000 13:00</t>
+  </si>
+  <si>
+    <t>10.09.1982</t>
+  </si>
+  <si>
+    <t>Dude</t>
+  </si>
+  <si>
+    <t>Sir</t>
+  </si>
+  <si>
+    <t>Garbage</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Diesel fuel</t>
+  </si>
+  <si>
+    <t>Stern</t>
+  </si>
+  <si>
+    <t>Crew change</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Haram</t>
+  </si>
+  <si>
+    <t>Steinar</t>
+  </si>
+  <si>
+    <t>Det Kalde Nord</t>
   </si>
 </sst>
 </file>
@@ -8189,7 +8258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -9022,20 +9091,9 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -9043,6 +9101,37 @@
     </xf>
     <xf numFmtId="20" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -16808,26 +16897,26 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="229" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
-      <c r="G1" s="223"/>
-      <c r="H1" s="223"/>
-      <c r="I1" s="223"/>
-      <c r="J1" s="223"/>
-      <c r="K1" s="223"/>
-      <c r="L1" s="223"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="223"/>
-      <c r="O1" s="223"/>
-      <c r="P1" s="223"/>
-      <c r="Q1" s="223"/>
-      <c r="R1" s="223"/>
+      <c r="B1" s="229"/>
+      <c r="C1" s="229"/>
+      <c r="D1" s="229"/>
+      <c r="E1" s="229"/>
+      <c r="F1" s="229"/>
+      <c r="G1" s="229"/>
+      <c r="H1" s="229"/>
+      <c r="I1" s="229"/>
+      <c r="J1" s="229"/>
+      <c r="K1" s="229"/>
+      <c r="L1" s="229"/>
+      <c r="M1" s="229"/>
+      <c r="N1" s="229"/>
+      <c r="O1" s="229"/>
+      <c r="P1" s="229"/>
+      <c r="Q1" s="229"/>
+      <c r="R1" s="229"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -16986,7 +17075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8:C8"/>
     </sheetView>
@@ -17198,10 +17287,10 @@
       <c r="A8" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="B8" s="224">
+      <c r="B8" s="221">
         <v>42685</v>
       </c>
-      <c r="C8" s="225">
+      <c r="C8" s="222">
         <v>0.46597222222222223</v>
       </c>
       <c r="D8" s="78"/>
@@ -17551,9 +17640,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18048,7 +18137,7 @@
       <c r="C8" s="5" t="s">
         <v>1386</v>
       </c>
-      <c r="D8" s="222" t="s">
+      <c r="D8" s="223" t="s">
         <v>1385</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -18088,8 +18177,8 @@
       <c r="C9" s="5" t="s">
         <v>1386</v>
       </c>
-      <c r="D9" s="220">
-        <v>36892.042372685188</v>
+      <c r="D9" s="224" t="s">
+        <v>1404</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>1392</v>
@@ -18137,7 +18226,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18587,16 +18676,36 @@
       </c>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="69" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="223">
+        <v>21641</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="5">
+        <v>345324534</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="K8" s="117">
         <v>1</v>
       </c>
@@ -18610,16 +18719,36 @@
       <c r="S8" s="60"/>
     </row>
     <row r="9" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="5" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="223">
+        <v>23605</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="5">
+        <v>323452345</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="K9" s="5">
         <v>2</v>
       </c>
@@ -18633,16 +18762,36 @@
       <c r="S9" s="60"/>
     </row>
     <row r="10" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="223">
+        <v>26825</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="5">
+        <v>23542354</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1402</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1392</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>1403</v>
+      </c>
       <c r="K10" s="5">
         <v>3</v>
       </c>
@@ -18656,16 +18805,36 @@
       <c r="S10" s="60"/>
     </row>
     <row r="11" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="5" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D11" s="224" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1391</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="5">
+        <v>123434563456</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1365</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>777</v>
+      </c>
       <c r="K11" s="5">
         <v>4</v>
       </c>
@@ -19247,9 +19416,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19682,13 +19851,27 @@
       </c>
     </row>
     <row r="8" spans="1:19" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="A8" s="69" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D8" s="230">
+        <v>30682</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="10">
+        <v>123456789</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="69">
@@ -20315,7 +20498,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20621,12 +20804,18 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="5" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B8" s="9">
+        <v>10</v>
+      </c>
       <c r="C8" s="119">
         <v>1</v>
       </c>
-      <c r="D8" s="56"/>
+      <c r="D8" s="56" t="s">
+        <v>639</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="59"/>
       <c r="G8" s="6"/>
@@ -20952,7 +21141,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21320,15 +21509,33 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="79"/>
+      <c r="A8" s="5" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1100</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D8" s="5">
+        <v>10</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>10</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="H8" s="9">
+        <v>10</v>
+      </c>
+      <c r="I8" s="225">
+        <v>42736.416666666664</v>
+      </c>
       <c r="J8" s="208"/>
       <c r="K8" s="120"/>
       <c r="L8" s="120"/>
@@ -21735,7 +21942,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22201,14 +22408,30 @@
       </c>
     </row>
     <row r="8" spans="1:27" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="78"/>
+      <c r="A8" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="226">
+        <v>42005</v>
+      </c>
+      <c r="C8" s="80">
+        <v>5001</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>1409</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G8" s="9">
+        <v>10</v>
+      </c>
+      <c r="H8" s="78">
+        <v>8</v>
+      </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -23045,7 +23268,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23623,10 +23846,10 @@
       <c r="N14" s="60"/>
     </row>
     <row r="15" spans="1:27" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="221" t="s">
+      <c r="A15" s="220" t="s">
         <v>1359</v>
       </c>
-      <c r="B15" s="221" t="s">
+      <c r="B15" s="220" t="s">
         <v>1360</v>
       </c>
       <c r="C15" s="218" t="s">
@@ -23649,10 +23872,10 @@
       <c r="N15" s="60"/>
     </row>
     <row r="16" spans="1:27" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="221" t="s">
+      <c r="A16" s="220" t="s">
         <v>1364</v>
       </c>
-      <c r="B16" s="221">
+      <c r="B16" s="220">
         <v>42305</v>
       </c>
       <c r="C16" s="218" t="s">
@@ -23675,10 +23898,10 @@
       <c r="N16" s="60"/>
     </row>
     <row r="17" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="221" t="s">
+      <c r="A17" s="220" t="s">
         <v>1367</v>
       </c>
-      <c r="B17" s="221">
+      <c r="B17" s="220">
         <v>42303</v>
       </c>
       <c r="C17" s="218" t="s">
@@ -23701,10 +23924,10 @@
       <c r="N17" s="60"/>
     </row>
     <row r="18" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="221" t="s">
+      <c r="A18" s="220" t="s">
         <v>1371</v>
       </c>
-      <c r="B18" s="221">
+      <c r="B18" s="220">
         <v>42301</v>
       </c>
       <c r="C18" s="218" t="s">
@@ -23727,10 +23950,10 @@
       <c r="N18" s="60"/>
     </row>
     <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="221" t="s">
+      <c r="A19" s="220" t="s">
         <v>1374</v>
       </c>
-      <c r="B19" s="221">
+      <c r="B19" s="220">
         <v>42299</v>
       </c>
       <c r="C19" s="218" t="s">
@@ -23753,10 +23976,10 @@
       <c r="N19" s="60"/>
     </row>
     <row r="20" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="221" t="s">
+      <c r="A20" s="220" t="s">
         <v>1378</v>
       </c>
-      <c r="B20" s="221">
+      <c r="B20" s="220">
         <v>42297</v>
       </c>
       <c r="C20" s="218" t="s">
@@ -23779,10 +24002,10 @@
       <c r="N20" s="60"/>
     </row>
     <row r="21" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="221" t="s">
+      <c r="A21" s="220" t="s">
         <v>1381</v>
       </c>
-      <c r="B21" s="221">
+      <c r="B21" s="220">
         <v>42227.416666666664</v>
       </c>
       <c r="C21" s="218" t="s">
@@ -23805,10 +24028,10 @@
       <c r="N21" s="60"/>
     </row>
     <row r="22" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="221" t="s">
+      <c r="A22" s="220" t="s">
         <v>1383</v>
       </c>
-      <c r="B22" s="221" t="s">
+      <c r="B22" s="220" t="s">
         <v>1384</v>
       </c>
       <c r="C22" s="218" t="s">
@@ -23831,10 +24054,10 @@
       <c r="N22" s="60"/>
     </row>
     <row r="23" spans="1:14" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="221" t="s">
+      <c r="A23" s="220" t="s">
         <v>1381</v>
       </c>
-      <c r="B23" s="221" t="s">
+      <c r="B23" s="220" t="s">
         <v>1382</v>
       </c>
       <c r="C23" s="218" t="s">
@@ -23857,10 +24080,10 @@
       <c r="N23" s="60"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="221" t="s">
+      <c r="A24" s="220" t="s">
         <v>1383</v>
       </c>
-      <c r="B24" s="221" t="s">
+      <c r="B24" s="220" t="s">
         <v>1384</v>
       </c>
       <c r="C24" s="218" t="s">
@@ -23961,13 +24184,27 @@
       <c r="N27" s="60"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="14"/>
+      <c r="A28" s="21">
+        <v>42305</v>
+      </c>
+      <c r="B28" s="21">
+        <v>42306</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D28" s="227">
+        <v>1</v>
+      </c>
+      <c r="E28" s="228">
+        <v>2</v>
+      </c>
+      <c r="F28" s="45" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>110</v>
+      </c>
       <c r="H28" s="5"/>
       <c r="I28" s="61"/>
       <c r="J28" s="57"/>
@@ -23980,8 +24217,8 @@
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="65"/>
+      <c r="D29" s="227"/>
+      <c r="E29" s="228"/>
       <c r="F29" s="26"/>
       <c r="G29" s="14"/>
       <c r="H29" s="5"/>
@@ -23996,8 +24233,8 @@
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="65"/>
+      <c r="D30" s="227"/>
+      <c r="E30" s="228"/>
       <c r="F30" s="26"/>
       <c r="G30" s="14"/>
       <c r="H30" s="5"/>
@@ -24012,8 +24249,8 @@
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="65"/>
+      <c r="D31" s="227"/>
+      <c r="E31" s="228"/>
       <c r="F31" s="26"/>
       <c r="G31" s="14"/>
       <c r="H31" s="5"/>
@@ -24028,8 +24265,8 @@
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="65"/>
+      <c r="D32" s="227"/>
+      <c r="E32" s="228"/>
       <c r="F32" s="26"/>
       <c r="G32" s="14"/>
       <c r="H32" s="5"/>
@@ -24044,8 +24281,8 @@
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="65"/>
+      <c r="D33" s="227"/>
+      <c r="E33" s="228"/>
       <c r="F33" s="26"/>
       <c r="G33" s="14"/>
       <c r="H33" s="5"/>
@@ -24060,8 +24297,8 @@
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="65"/>
+      <c r="D34" s="227"/>
+      <c r="E34" s="228"/>
       <c r="F34" s="26"/>
       <c r="G34" s="14"/>
       <c r="H34" s="5"/>
@@ -24076,8 +24313,8 @@
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="65"/>
+      <c r="D35" s="227"/>
+      <c r="E35" s="228"/>
       <c r="F35" s="26"/>
       <c r="G35" s="14"/>
       <c r="H35" s="5"/>
@@ -24092,8 +24329,8 @@
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="65"/>
+      <c r="D36" s="227"/>
+      <c r="E36" s="228"/>
       <c r="F36" s="26"/>
       <c r="G36" s="14"/>
       <c r="H36" s="5"/>
@@ -24108,8 +24345,8 @@
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="65"/>
+      <c r="D37" s="227"/>
+      <c r="E37" s="228"/>
       <c r="F37" s="26"/>
       <c r="G37" s="14"/>
       <c r="H37" s="5"/>
@@ -24124,8 +24361,8 @@
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="65"/>
+      <c r="D38" s="227"/>
+      <c r="E38" s="228"/>
       <c r="F38" s="26"/>
       <c r="G38" s="14"/>
       <c r="H38" s="5"/>
@@ -24140,8 +24377,8 @@
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="65"/>
+      <c r="D39" s="227"/>
+      <c r="E39" s="228"/>
       <c r="F39" s="26"/>
       <c r="G39" s="14"/>
       <c r="H39" s="5"/>
@@ -24156,8 +24393,8 @@
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="65"/>
+      <c r="D40" s="227"/>
+      <c r="E40" s="228"/>
       <c r="F40" s="26"/>
       <c r="G40" s="14"/>
       <c r="H40" s="5"/>
@@ -24172,8 +24409,8 @@
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="65"/>
+      <c r="D41" s="227"/>
+      <c r="E41" s="228"/>
       <c r="F41" s="26"/>
       <c r="G41" s="14"/>
     </row>

</xml_diff>

<commit_message>
Added typed sheets for crew/pax and waste.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arrival_Or_Departure" sheetId="2" r:id="rId1"/>
@@ -2214,7 +2214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="1417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1425">
   <si>
     <t>Port call</t>
   </si>
@@ -7243,6 +7243,30 @@
   </si>
   <si>
     <t>Det Kalde Nord</t>
+  </si>
+  <si>
+    <t>Ravnestad</t>
+  </si>
+  <si>
+    <t>Andreas</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Førde</t>
+  </si>
+  <si>
+    <t>Vaskehjelp</t>
+  </si>
+  <si>
+    <t>Rofle</t>
+  </si>
+  <si>
+    <t>Snofle</t>
+  </si>
+  <si>
+    <t>500.10</t>
   </si>
 </sst>
 </file>
@@ -8258,7 +8282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="231">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -9127,12 +9151,16 @@
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -16897,26 +16925,26 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="229" t="s">
+      <c r="A1" s="231" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="229"/>
-      <c r="L1" s="229"/>
-      <c r="M1" s="229"/>
-      <c r="N1" s="229"/>
-      <c r="O1" s="229"/>
-      <c r="P1" s="229"/>
-      <c r="Q1" s="229"/>
-      <c r="R1" s="229"/>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="231"/>
+      <c r="I1" s="231"/>
+      <c r="J1" s="231"/>
+      <c r="K1" s="231"/>
+      <c r="L1" s="231"/>
+      <c r="M1" s="231"/>
+      <c r="N1" s="231"/>
+      <c r="O1" s="231"/>
+      <c r="P1" s="231"/>
+      <c r="Q1" s="231"/>
+      <c r="R1" s="231"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -17638,11 +17666,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18206,6 +18234,52 @@
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
       <c r="V9" s="60"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G10" s="1">
+        <v>91700891</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G11" s="1">
+        <v>91700891</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="I11" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <protectedRanges>
@@ -19416,7 +19490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
@@ -19860,7 +19934,7 @@
       <c r="C8" s="56" t="s">
         <v>1386</v>
       </c>
-      <c r="D8" s="230">
+      <c r="D8" s="229">
         <v>30682</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -21141,7 +21215,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21518,11 +21592,11 @@
       <c r="C8" s="5" t="s">
         <v>1409</v>
       </c>
-      <c r="D8" s="5">
-        <v>10</v>
+      <c r="D8" s="230" t="s">
+        <v>1424</v>
       </c>
       <c r="E8" s="5">
-        <v>10</v>
+        <v>20.5</v>
       </c>
       <c r="F8" s="5">
         <v>10</v>
@@ -21544,7 +21618,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="230"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -21558,7 +21632,7 @@
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="230"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -21572,7 +21646,7 @@
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="230"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -21586,7 +21660,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="230"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -21600,7 +21674,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="230"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -21614,7 +21688,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="230"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -21628,7 +21702,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="230"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -21642,7 +21716,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="230"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -21656,7 +21730,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="230"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -21670,7 +21744,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="230"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -21684,7 +21758,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="230"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -21698,7 +21772,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="230"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -21712,7 +21786,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="230"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -21726,7 +21800,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="D22" s="230"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -21740,7 +21814,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="D23" s="230"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -21754,7 +21828,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="D24" s="230"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -21768,7 +21842,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="230"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -21782,7 +21856,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="230"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -21796,7 +21870,7 @@
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="230"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -21810,7 +21884,7 @@
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="230"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -21824,7 +21898,7 @@
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="230"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -21838,7 +21912,7 @@
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="230"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -21852,7 +21926,7 @@
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="230"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -21866,7 +21940,7 @@
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="230"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -21880,7 +21954,7 @@
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="230"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -21894,7 +21968,7 @@
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="230"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -21908,7 +21982,7 @@
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="230"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>

</xml_diff>

<commit_message>
Improved type detection and conversion.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14880" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Arrival_Or_Departure" sheetId="2" r:id="rId1"/>
@@ -2214,7 +2214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="1431">
   <si>
     <t>Port call</t>
   </si>
@@ -7267,6 +7267,24 @@
   </si>
   <si>
     <t>500.10</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>whatever</t>
+  </si>
+  <si>
+    <t>Dings</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>###</t>
   </si>
 </sst>
 </file>
@@ -8282,7 +8300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="233">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -9162,6 +9180,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9554,11 +9576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10485,22 +10507,52 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C8" s="5">
+        <v>123</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E8" s="232">
+        <v>42342.458333333336</v>
+      </c>
+      <c r="F8" s="232">
+        <v>42342.5</v>
+      </c>
+      <c r="G8" s="232">
+        <v>42342.666666666664</v>
+      </c>
+      <c r="H8" s="232">
+        <v>42342.666666666664</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>1427</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1</v>
+      </c>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="9"/>
+      <c r="L8" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="N8" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="P8" s="9">
+        <v>123456789</v>
+      </c>
       <c r="Q8" s="56"/>
       <c r="R8" s="10"/>
       <c r="S8" s="59"/>
@@ -10509,11 +10561,105 @@
       <c r="V8" s="10"/>
       <c r="W8" s="97"/>
     </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>1372</v>
+      </c>
+      <c r="E9" s="232"/>
+      <c r="F9" s="232">
+        <v>42342.5</v>
+      </c>
+      <c r="G9" s="232">
+        <v>42342.666666666664</v>
+      </c>
+      <c r="H9" s="232">
+        <v>42342.666666666664</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>1427</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>1428</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>1418</v>
+      </c>
+      <c r="P9" s="9">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>1430</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>1430</v>
+      </c>
+    </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="D8:P8" name="Område1_3"/>
     <protectedRange sqref="T8:W8" name="Område1"/>
     <protectedRange sqref="Q8:S8" name="Område1_1"/>
+    <protectedRange sqref="D8:P9" name="Område1_3_1"/>
   </protectedRanges>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="http://www.annamsw.eu/news/151-anna-spread-sheet-template-nearly-ready.html"/>
@@ -17668,7 +17814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>

</xml_diff>

<commit_message>
Added support for removing empty rows from strongly typed sheets. Still needs some performance testing and possibly improvement.
</commit_message>
<xml_diff>
--- a/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
+++ b/src/AnNaSpreadsheetParser.Test/AnNaTestSheet.xlsx
@@ -9177,12 +9177,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="22" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9580,7 +9580,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:P10"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9588,7 +9588,9 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="8" width="16.7109375" customWidth="1"/>
+    <col min="4" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -10519,16 +10521,16 @@
       <c r="D8" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="E8" s="232">
+      <c r="E8" s="231">
         <v>42342.458333333336</v>
       </c>
-      <c r="F8" s="232">
+      <c r="F8" s="231">
         <v>42342.5</v>
       </c>
-      <c r="G8" s="232">
+      <c r="G8" s="231">
         <v>42342.666666666664</v>
       </c>
-      <c r="H8" s="232">
+      <c r="H8" s="231">
         <v>42342.666666666664</v>
       </c>
       <c r="I8" s="5" t="s">
@@ -10572,14 +10574,14 @@
       <c r="D9" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232">
+      <c r="E9" s="231"/>
+      <c r="F9" s="231">
         <v>42342.5</v>
       </c>
-      <c r="G9" s="232">
+      <c r="G9" s="231">
         <v>42342.666666666664</v>
       </c>
-      <c r="H9" s="232">
+      <c r="H9" s="231">
         <v>42342.666666666664</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -17071,26 +17073,26 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="231" t="s">
+      <c r="A1" s="232" t="s">
         <v>1151</v>
       </c>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
-      <c r="N1" s="231"/>
-      <c r="O1" s="231"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="R1" s="231"/>
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
+      <c r="H1" s="232"/>
+      <c r="I1" s="232"/>
+      <c r="J1" s="232"/>
+      <c r="K1" s="232"/>
+      <c r="L1" s="232"/>
+      <c r="M1" s="232"/>
+      <c r="N1" s="232"/>
+      <c r="O1" s="232"/>
+      <c r="P1" s="232"/>
+      <c r="Q1" s="232"/>
+      <c r="R1" s="232"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">

</xml_diff>